<commit_message>
Update formulas and functions
</commit_message>
<xml_diff>
--- a/Lessons/Lesson03/Lesson03_Homework.xlsx
+++ b/Lessons/Lesson03/Lesson03_Homework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/afb04e5a841adf33/Documents/GitHub/IntroToExcel/Lessons/Lesson03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="8_{A8CC901F-3301-4E59-80E1-69C65C475832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4131246F-0CCF-4E03-B55B-E912AEBEB3E6}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="8_{A8CC901F-3301-4E59-80E1-69C65C475832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E9007511-8BF1-4F18-9AF3-1921E2D3635E}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{B743010D-C9DF-4FB9-B797-0F3970CDB3F7}"/>
   </bookViews>
@@ -195,12 +195,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -275,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -283,11 +289,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +667,7 @@
   <dimension ref="A12:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
@@ -673,8 +680,8 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:15" ht="25.8" x14ac:dyDescent="0.95">
       <c r="A14" s="1" t="s">
@@ -688,76 +695,76 @@
     </row>
     <row r="16" spans="1:15" ht="13.2" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
+      <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="9"/>
+      <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -785,7 +792,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.87890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.29296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">

</xml_diff>